<commit_message>
updated sprint backlog and burndown chart again
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint 1/Sprint Backlog.xlsx
+++ b/Project/Phase 1/Sprint 1/Sprint Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GonVirginia\IdeaProjects\SE2122_55677_56773__56971_57066_58655\Project\Phase 1\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C8ADC-381B-46B5-8BB5-D68B7320B204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF8EE51-24E5-4C8B-965C-14EB5B0B0883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="1605" windowWidth="21600" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="1530" windowWidth="21600" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A15" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>